<commit_message>
fixed:  extract endpoint to process requirement text and URL, with new schema
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="30">
   <si>
     <t>Module</t>
   </si>
@@ -35,73 +35,61 @@
     <t>DevOps Days</t>
   </si>
   <si>
-    <t>Form</t>
-  </si>
-  <si>
-    <t>List of available Doctors</t>
-  </si>
-  <si>
-    <t>Context sensitive</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>List all shared files</t>
-  </si>
-  <si>
-    <t>Speciality</t>
-  </si>
-  <si>
-    <t>Other details</t>
-  </si>
-  <si>
-    <t>Search Doctor within radius</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>List of Clinics Doctor is available at - time and price</t>
-  </si>
-  <si>
-    <t>Confirm appointment with payment</t>
-  </si>
-  <si>
-    <t>Sync Smart watch</t>
+    <t>AI-Powered Proficiency Assessment</t>
+  </si>
+  <si>
+    <t>Adaptive Lesson Planning</t>
+  </si>
+  <si>
+    <t>Conversational AI for Real-Life Dialogues</t>
+  </si>
+  <si>
+    <t>Spaced Repetition &amp; Revision Scheduling</t>
+  </si>
+  <si>
+    <t>AI-Based Diagnostic Test</t>
+  </si>
+  <si>
+    <t>Ongoing Performance Analysis</t>
+  </si>
+  <si>
+    <t>Proficiency Display</t>
+  </si>
+  <si>
+    <t>Learning History Storage</t>
+  </si>
+  <si>
+    <t>AI Component</t>
+  </si>
+  <si>
+    <t>Personalized Lesson Plans</t>
+  </si>
+  <si>
+    <t>Interactive Lesson Display</t>
+  </si>
+  <si>
+    <t>Lesson Data Management</t>
+  </si>
+  <si>
+    <t>Real-World Conversation Simulation</t>
+  </si>
+  <si>
+    <t>Chat-Based Conversational UI</t>
+  </si>
+  <si>
+    <t>Conversation Data Processing</t>
+  </si>
+  <si>
+    <t>AI-Powered Revision Schedules</t>
+  </si>
+  <si>
+    <t>Timely Lesson Reminders</t>
+  </si>
+  <si>
+    <t>Past Lessons Logging</t>
   </si>
   <si>
     <t>Development</t>
-  </si>
-  <si>
-    <t>View Privacy Policy</t>
-  </si>
-  <si>
-    <t>View Terms &amp; Conditions</t>
-  </si>
-  <si>
-    <t>View App Info</t>
-  </si>
-  <si>
-    <t>View Disclaimer</t>
-  </si>
-  <si>
-    <t>Add/delete photo and text</t>
-  </si>
-  <si>
-    <t>View and update profile</t>
-  </si>
-  <si>
-    <t>Subscription status</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>View shared file</t>
   </si>
   <si>
     <t>Testing</t>
@@ -474,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -505,19 +493,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E2">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -525,16 +513,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -545,19 +533,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -565,16 +553,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -585,19 +573,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="F6">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -605,30 +593,30 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="F7">
-        <v>0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -642,13 +630,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -662,22 +650,22 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>0.27</v>
+        <v>0.36</v>
       </c>
       <c r="F10">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -685,19 +673,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0.18</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -705,19 +693,19 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -725,19 +713,19 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
         <v>0.09</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -745,19 +733,19 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>0.36</v>
+        <v>0.09</v>
       </c>
       <c r="F14">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -765,90 +753,90 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E15">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>0.36</v>
+        <v>0.09</v>
       </c>
       <c r="F16">
-        <v>0.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>0.18</v>
+        <v>0.36</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E18">
-        <v>0.09</v>
+        <v>0.27</v>
       </c>
       <c r="F18">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -862,33 +850,33 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F20">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -902,13 +890,13 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -922,13 +910,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -942,22 +930,22 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>0.09</v>
+        <v>0.36</v>
       </c>
       <c r="F24">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -965,273 +953,153 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E27">
         <v>0.09</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0.09</v>
       </c>
       <c r="F28">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
         <v>0.09</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E30">
         <v>0.09</v>
       </c>
       <c r="F30">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>0.36</v>
+      </c>
+      <c r="F31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0.09</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
       <c r="D32">
-        <v>0.5</v>
+        <v>18.5</v>
       </c>
       <c r="E32">
-        <v>0.09</v>
+        <v>4.409999999999999</v>
       </c>
       <c r="F32">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0.09</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>0.18</v>
-      </c>
-      <c r="F34">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0.09</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36">
-        <v>0.5</v>
-      </c>
-      <c r="E36">
-        <v>0.09</v>
-      </c>
-      <c r="F36">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0.09</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38">
-        <v>13.7</v>
-      </c>
-      <c r="E38">
-        <v>6.049999999999999</v>
-      </c>
-      <c r="F38">
-        <v>2.97</v>
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>
@@ -1241,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1261,19 +1129,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1281,28 +1149,28 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F2">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1310,10 +1178,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1322,10 +1190,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1339,28 +1207,28 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1368,10 +1236,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1380,10 +1248,10 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1397,28 +1265,28 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>9</v>
       </c>
       <c r="H6">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1426,39 +1294,39 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H7">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>0.5</v>
@@ -1481,13 +1349,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1510,31 +1378,31 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="F10">
-        <v>0.27</v>
+        <v>0.36</v>
       </c>
       <c r="G10">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="H10">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="I10">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1542,16 +1410,16 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F11">
         <v>0.18</v>
@@ -1560,10 +1428,10 @@
         <v>18</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1571,28 +1439,28 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="G12">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H12">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1600,16 +1468,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F13">
         <v>0.09</v>
@@ -1618,10 +1486,10 @@
         <v>9</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1629,28 +1497,28 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0.36</v>
+        <v>0.09</v>
       </c>
       <c r="G14">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="H14">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1658,126 +1526,126 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F15">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="G15">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0.36</v>
+        <v>0.09</v>
       </c>
       <c r="G16">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="H16">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F17">
-        <v>0.18</v>
+        <v>0.36</v>
       </c>
       <c r="G17">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F18">
-        <v>0.09</v>
+        <v>0.27</v>
       </c>
       <c r="G18">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="H18">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I18">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1800,42 +1668,42 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F20">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="G20">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H20">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I20">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1858,13 +1726,13 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>0.5</v>
@@ -1887,13 +1755,13 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1916,31 +1784,31 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="F24">
-        <v>0.09</v>
+        <v>0.36</v>
       </c>
       <c r="G24">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="H24">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="I24">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1948,74 +1816,74 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F25">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="G25">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="G26">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H26">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F27">
         <v>0.09</v>
@@ -2024,27 +1892,27 @@
         <v>9</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0.09</v>
@@ -2053,27 +1921,27 @@
         <v>9</v>
       </c>
       <c r="H28">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I28">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F29">
         <v>0.09</v>
@@ -2082,27 +1950,27 @@
         <v>9</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0.09</v>
@@ -2111,236 +1979,62 @@
         <v>9</v>
       </c>
       <c r="H30">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>400</v>
+      </c>
+      <c r="F31">
+        <v>0.36</v>
+      </c>
+      <c r="G31">
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <v>0.4</v>
+      </c>
+      <c r="I31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="C32" t="s">
         <v>26</v>
       </c>
-      <c r="C31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0.09</v>
-      </c>
-      <c r="G31">
-        <v>9</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
       <c r="D32">
-        <v>0.5</v>
+        <v>18.5</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>3700</v>
       </c>
       <c r="F32">
-        <v>0.09</v>
+        <v>4.409999999999999</v>
       </c>
       <c r="G32">
-        <v>9</v>
+        <v>441</v>
       </c>
       <c r="H32">
-        <v>0.1</v>
+        <v>3.6</v>
       </c>
       <c r="I32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>0.09</v>
-      </c>
-      <c r="G33">
-        <v>9</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>200</v>
-      </c>
-      <c r="F34">
-        <v>0.18</v>
-      </c>
-      <c r="G34">
-        <v>18</v>
-      </c>
-      <c r="H34">
-        <v>0.2</v>
-      </c>
-      <c r="I34">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0.09</v>
-      </c>
-      <c r="G35">
-        <v>9</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36">
-        <v>0.5</v>
-      </c>
-      <c r="E36">
-        <v>100</v>
-      </c>
-      <c r="F36">
-        <v>0.09</v>
-      </c>
-      <c r="G36">
-        <v>9</v>
-      </c>
-      <c r="H36">
-        <v>0.1</v>
-      </c>
-      <c r="I36">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0.09</v>
-      </c>
-      <c r="G37">
-        <v>9</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38">
-        <v>13.7</v>
-      </c>
-      <c r="E38">
-        <v>2740</v>
-      </c>
-      <c r="F38">
-        <v>6.049999999999999</v>
-      </c>
-      <c r="G38">
-        <v>605</v>
-      </c>
-      <c r="H38">
-        <v>2.97</v>
-      </c>
-      <c r="I38">
-        <v>891</v>
+        <v>1080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add tech stack and platform fields to requirement extraction
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="36">
   <si>
     <t>Module</t>
   </si>
@@ -29,82 +29,100 @@
     <t>Dev Days</t>
   </si>
   <si>
+    <t>Dev Buffer</t>
+  </si>
+  <si>
     <t>Test Days</t>
   </si>
   <si>
     <t>DevOps Days</t>
   </si>
   <si>
-    <t>AI-Powered Proficiency Assessment</t>
-  </si>
-  <si>
-    <t>Adaptive Lesson Planning</t>
-  </si>
-  <si>
-    <t>Conversational AI for Real-Life Dialogues</t>
-  </si>
-  <si>
-    <t>Spaced Repetition &amp; Revision Scheduling</t>
-  </si>
-  <si>
-    <t>AI-Based Diagnostic Test</t>
-  </si>
-  <si>
-    <t>Ongoing Performance Analysis</t>
-  </si>
-  <si>
-    <t>Proficiency Display</t>
-  </si>
-  <si>
-    <t>Learning History Storage</t>
-  </si>
-  <si>
-    <t>AI Component</t>
-  </si>
-  <si>
-    <t>Personalized Lesson Plans</t>
-  </si>
-  <si>
-    <t>Interactive Lesson Display</t>
-  </si>
-  <si>
-    <t>Lesson Data Management</t>
-  </si>
-  <si>
-    <t>Real-World Conversation Simulation</t>
-  </si>
-  <si>
-    <t>Chat-Based Conversational UI</t>
-  </si>
-  <si>
-    <t>Conversation Data Processing</t>
-  </si>
-  <si>
-    <t>AI-Powered Revision Schedules</t>
-  </si>
-  <si>
-    <t>Timely Lesson Reminders</t>
-  </si>
-  <si>
-    <t>Past Lessons Logging</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>Testing</t>
+    <t>Patient Mobile Application</t>
+  </si>
+  <si>
+    <t>Doctor Mobile Application</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Dev Cost</t>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>List of available Doctors</t>
+  </si>
+  <si>
+    <t>Context sensitive</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Speciality</t>
+  </si>
+  <si>
+    <t>Other details</t>
+  </si>
+  <si>
+    <t>Search Doctor within radius</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>List of Clinics Doctor is available at - time and price</t>
+  </si>
+  <si>
+    <t>Confirm appointment with payment</t>
+  </si>
+  <si>
+    <t>Sync Smart watch</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>View Privacy Policy</t>
+  </si>
+  <si>
+    <t>View Terms &amp; Conditions</t>
+  </si>
+  <si>
+    <t>View App Info</t>
+  </si>
+  <si>
+    <t>View Disclaimer</t>
+  </si>
+  <si>
+    <t>Add/delete photo and text</t>
+  </si>
+  <si>
+    <t>View and update profile</t>
+  </si>
+  <si>
+    <t>Subscription status</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>days</t>
   </si>
   <si>
     <t>Test Cost</t>
   </si>
   <si>
     <t>DevOps Cost</t>
+  </si>
+  <si>
+    <t>INR</t>
   </si>
 </sst>
 </file>
@@ -462,13 +480,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,619 +505,758 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>0.18</v>
       </c>
-      <c r="F4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E6">
-        <v>0.09</v>
+        <v>0.3</v>
       </c>
       <c r="F6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>0.36</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>0.24</v>
+      </c>
+      <c r="G7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.48</v>
+      </c>
+      <c r="G8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>0.12</v>
+      </c>
+      <c r="G9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>0.5</v>
-      </c>
-      <c r="E8">
-        <v>0.09</v>
-      </c>
-      <c r="F8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0.09</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0.12</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>0.1</v>
+      </c>
+      <c r="F11">
+        <v>0.12</v>
+      </c>
+      <c r="G11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <v>0.1</v>
+      </c>
+      <c r="F12">
+        <v>0.12</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>0.1</v>
+      </c>
+      <c r="F13">
+        <v>0.12</v>
+      </c>
+      <c r="G13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.2</v>
+      </c>
+      <c r="F14">
+        <v>0.24</v>
+      </c>
+      <c r="G14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+      <c r="E15">
+        <v>0.1</v>
+      </c>
+      <c r="F15">
+        <v>0.12</v>
+      </c>
+      <c r="G15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>0.1</v>
+      </c>
+      <c r="F16">
+        <v>0.12</v>
+      </c>
+      <c r="G16">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>0.1</v>
+      </c>
+      <c r="F17">
+        <v>0.12</v>
+      </c>
+      <c r="G17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>0.1</v>
+      </c>
+      <c r="F18">
+        <v>0.12</v>
+      </c>
+      <c r="G18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
+      </c>
+      <c r="F20">
+        <v>0.12</v>
+      </c>
+      <c r="G20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>1.5</v>
+      </c>
+      <c r="E21">
+        <v>0.3</v>
+      </c>
+      <c r="F21">
+        <v>0.36</v>
+      </c>
+      <c r="G21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>0.24</v>
+      </c>
+      <c r="G22">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="E10">
-        <v>0.36</v>
-      </c>
-      <c r="F10">
+      <c r="E23">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0.18</v>
-      </c>
-      <c r="F11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0.09</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13">
-        <v>0.5</v>
-      </c>
-      <c r="E13">
-        <v>0.09</v>
-      </c>
-      <c r="F13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0.09</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15">
-        <v>0.09</v>
-      </c>
-      <c r="F15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0.09</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>0.36</v>
-      </c>
-      <c r="F17">
+      <c r="F23">
+        <v>0.48</v>
+      </c>
+      <c r="G23">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18">
-        <v>1.5</v>
-      </c>
-      <c r="E18">
-        <v>0.27</v>
-      </c>
-      <c r="F18">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0.09</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>0.18</v>
-      </c>
-      <c r="F20">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0.09</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
-      </c>
-      <c r="E22">
-        <v>0.09</v>
-      </c>
-      <c r="F22">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0.09</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E24">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="F24">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="F25">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E26">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G26">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <v>0.5</v>
       </c>
       <c r="E27">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F27">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D29">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="F29">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>0.24</v>
+      </c>
+      <c r="G29">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E30">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G30">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E31">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="F31">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>0.12</v>
+      </c>
+      <c r="G31">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>18.5</v>
+        <v>0.5</v>
       </c>
       <c r="E32">
-        <v>4.409999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
-        <v>3.6</v>
+        <v>0.12</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>4.199999999999999</v>
+      </c>
+      <c r="F33">
+        <v>5.040000000000001</v>
+      </c>
+      <c r="G33">
+        <v>3.860000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1109,7 +1266,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1129,59 +1286,59 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="G2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I2">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1190,10 +1347,10 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1204,205 +1361,205 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.18</v>
       </c>
-      <c r="G4">
-        <v>18</v>
-      </c>
-      <c r="H4">
-        <v>0.2</v>
-      </c>
       <c r="I4">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>0.3</v>
       </c>
       <c r="F6">
-        <v>0.09</v>
+        <v>0.36</v>
       </c>
       <c r="G6">
-        <v>9</v>
+        <v>36.00000000000001</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
-        <v>0.09</v>
+        <v>0.24</v>
       </c>
       <c r="G7">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
-        <v>0.09</v>
+        <v>0.48</v>
       </c>
       <c r="G8">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="H8">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F9">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G9">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
-        <v>400</v>
+        <v>0.1</v>
       </c>
       <c r="F10">
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="G10">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I10">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1410,28 +1567,28 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>200</v>
+        <v>0.1</v>
       </c>
       <c r="F11">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="G11">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I11">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1439,28 +1596,28 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F12">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1468,22 +1625,22 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>0.5</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F13">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G13">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H13">
         <v>0.1</v>
@@ -1497,28 +1654,28 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F14">
-        <v>0.09</v>
+        <v>0.24</v>
       </c>
       <c r="G14">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1526,22 +1683,22 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>0.5</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F15">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G15">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <v>0.1</v>
@@ -1555,28 +1712,28 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F16">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G16">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1584,28 +1741,28 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E17">
-        <v>400</v>
+        <v>0.1</v>
       </c>
       <c r="F17">
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="G17">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H17">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I17">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1613,28 +1770,28 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D18">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E18">
-        <v>300</v>
+        <v>0.1</v>
       </c>
       <c r="F18">
-        <v>0.27</v>
+        <v>0.12</v>
       </c>
       <c r="G18">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H18">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="I18">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1642,10 +1799,10 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1654,10 +1811,10 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1671,28 +1828,28 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
       <c r="D20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E20">
-        <v>200</v>
+        <v>0.1</v>
       </c>
       <c r="F20">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="G20">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H20">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I20">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1700,28 +1857,28 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F21">
-        <v>0.09</v>
+        <v>0.36</v>
       </c>
       <c r="G21">
-        <v>9</v>
+        <v>36.00000000000001</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1729,22 +1886,22 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.2</v>
+      </c>
+      <c r="F22">
+        <v>0.24</v>
+      </c>
+      <c r="G22">
         <v>24</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
-      </c>
-      <c r="E22">
-        <v>100</v>
-      </c>
-      <c r="F22">
-        <v>0.09</v>
-      </c>
-      <c r="G22">
-        <v>9</v>
       </c>
       <c r="H22">
         <v>0.1</v>
@@ -1758,28 +1915,28 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F23">
-        <v>0.09</v>
+        <v>0.48</v>
       </c>
       <c r="G23">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1787,109 +1944,109 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E24">
-        <v>400</v>
+        <v>0.1</v>
       </c>
       <c r="F24">
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="G24">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H24">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I24">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>200</v>
+        <v>0.1</v>
       </c>
       <c r="F25">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="G25">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H25">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I25">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F26">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G26">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27">
         <v>0.5</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="F27">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G27">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H27">
         <v>0.1</v>
@@ -1900,141 +2057,196 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F28">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G28">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0.2</v>
+      </c>
+      <c r="F29">
+        <v>0.24</v>
+      </c>
+      <c r="G29">
         <v>24</v>
       </c>
-      <c r="D29">
-        <v>0.5</v>
-      </c>
-      <c r="E29">
-        <v>100</v>
-      </c>
-      <c r="F29">
-        <v>0.09</v>
-      </c>
-      <c r="G29">
-        <v>9</v>
-      </c>
       <c r="H29">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I29">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="G30">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E31">
-        <v>400</v>
+        <v>0.1</v>
       </c>
       <c r="F31">
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="G31">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H31">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
       <c r="I31">
-        <v>120</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>18.5</v>
+        <v>0.5</v>
       </c>
       <c r="E32">
-        <v>3700</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
-        <v>4.409999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="G32">
-        <v>441</v>
+        <v>12</v>
       </c>
       <c r="H32">
-        <v>3.6</v>
+        <v>0.1</v>
       </c>
       <c r="I32">
-        <v>1080</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>21</v>
+      </c>
+      <c r="E33">
+        <v>4.199999999999999</v>
+      </c>
+      <c r="F33">
+        <v>5.040000000000001</v>
+      </c>
+      <c r="G33">
+        <v>504</v>
+      </c>
+      <c r="H33">
+        <v>3.860000000000001</v>
+      </c>
+      <c r="I33">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update wireframe generation to use selenium_pipeline and enhance tech stack recommendation logic
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Module</t>
   </si>
@@ -44,58 +44,52 @@
     <t>Backend Testing</t>
   </si>
   <si>
+    <t>Frontend Development</t>
+  </si>
+  <si>
+    <t>Backend Development</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>User Authentication</t>
   </si>
   <si>
-    <t>Product Management</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Sign Up</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Password Reset</t>
-  </si>
-  <si>
-    <t>Product Listing</t>
-  </si>
-  <si>
-    <t>Product Detail</t>
-  </si>
-  <si>
-    <t>Add Product</t>
-  </si>
-  <si>
-    <t>Edit Product</t>
-  </si>
-  <si>
-    <t>Form Validation</t>
-  </si>
-  <si>
-    <t>Password Hashing</t>
-  </si>
-  <si>
-    <t>Database Integration</t>
-  </si>
-  <si>
-    <t>Authentication API</t>
-  </si>
-  <si>
-    <t>Email Verification</t>
-  </si>
-  <si>
-    <t>Password Reset API</t>
-  </si>
-  <si>
-    <t>API Integration</t>
-  </si>
-  <si>
-    <t>UI/UX Implementation</t>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>User Management</t>
+  </si>
+  <si>
+    <t>Data Storage</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Registration Page</t>
+  </si>
+  <si>
+    <t>Password Recovery</t>
+  </si>
+  <si>
+    <t>Main Layout</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Data Mapping</t>
   </si>
   <si>
     <t>Units</t>
@@ -125,16 +119,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹5,068.80</t>
-  </si>
-  <si>
-    <t>₹4,899.84</t>
-  </si>
-  <si>
-    <t>₹608.26</t>
-  </si>
-  <si>
-    <t>₹10,576.90</t>
+    <t>₹4,435.20</t>
+  </si>
+  <si>
+    <t>₹8,785.92</t>
+  </si>
+  <si>
+    <t>₹532.22</t>
+  </si>
+  <si>
+    <t>₹13,753.34</t>
   </si>
 </sst>
 </file>
@@ -495,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -538,25 +532,25 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="G2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>0.6000000000000001</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>0.54</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>0.4</v>
-      </c>
-      <c r="I2">
-        <v>0.36</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -567,25 +561,25 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>0.2</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I3">
-        <v>0.18</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -596,16 +590,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -628,22 +622,22 @@
         <v>19</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="F5">
-        <v>0.36</v>
+        <v>1.26</v>
       </c>
       <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5">
-        <v>0.2</v>
-      </c>
       <c r="I5">
-        <v>0.18</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -654,25 +648,25 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
-        <v>0.2</v>
-      </c>
       <c r="F6">
-        <v>0.18</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I6">
-        <v>0.36</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -680,19 +674,19 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="F7">
-        <v>0.36</v>
+        <v>0.54</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -706,31 +700,31 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H8">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>0.36</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -738,28 +732,28 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H9">
-        <v>0.6000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="I9">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -767,28 +761,28 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -796,28 +790,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>0.4</v>
-      </c>
-      <c r="F11">
-        <v>0.36</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>0.4</v>
-      </c>
       <c r="I11">
-        <v>0.36</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -825,251 +819,77 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E13">
-        <v>0.6000000000000001</v>
+        <v>5.6</v>
       </c>
       <c r="F13">
-        <v>0.54</v>
+        <v>5.039999999999999</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="H13">
-        <v>0.4</v>
+        <v>10.4</v>
       </c>
       <c r="I13">
-        <v>0.36</v>
+        <v>9.359999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>0.4</v>
-      </c>
-      <c r="F14">
-        <v>0.36</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>0.4</v>
-      </c>
-      <c r="I14">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>0.4</v>
-      </c>
-      <c r="I15">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-      <c r="E16">
-        <v>0.4</v>
-      </c>
-      <c r="F16">
-        <v>0.36</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>0.4</v>
-      </c>
-      <c r="I16">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>0.4</v>
-      </c>
-      <c r="F17">
-        <v>0.36</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>0.4</v>
-      </c>
-      <c r="I17">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>0.4</v>
-      </c>
-      <c r="I18">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19">
-        <v>32</v>
-      </c>
-      <c r="E19">
-        <v>6.4</v>
-      </c>
-      <c r="F19">
-        <v>5.76</v>
-      </c>
-      <c r="G19">
-        <v>29</v>
-      </c>
-      <c r="H19">
-        <v>5.800000000000001</v>
-      </c>
-      <c r="I19">
-        <v>5.220000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1086,65 +906,65 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2">
-        <v>42.24</v>
+        <v>36.96</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3">
-        <v>38.28</v>
+        <v>68.64000000000001</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4">
-        <v>6.335999999999999</v>
+        <v>5.544</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1152,7 +972,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update file paths in effort estimation and wireframe generator scripts for better portability
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Module</t>
   </si>
@@ -44,52 +44,40 @@
     <t>Backend Testing</t>
   </si>
   <si>
-    <t>Frontend Development</t>
-  </si>
-  <si>
-    <t>Backend Development</t>
+    <t>User Authentication</t>
+  </si>
+  <si>
+    <t>Product Catalog</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>User Authentication</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
-    <t>User Management</t>
-  </si>
-  <si>
-    <t>Data Storage</t>
-  </si>
-  <si>
-    <t>Login Page</t>
-  </si>
-  <si>
-    <t>Registration Page</t>
-  </si>
-  <si>
-    <t>Password Recovery</t>
-  </si>
-  <si>
-    <t>Main Layout</t>
-  </si>
-  <si>
-    <t>User Profile</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
     <t>User Registration</t>
   </si>
   <si>
-    <t>Database Design</t>
-  </si>
-  <si>
-    <t>Data Mapping</t>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Product Listing</t>
+  </si>
+  <si>
+    <t>Product Details</t>
+  </si>
+  <si>
+    <t>Frontend Implementation</t>
+  </si>
+  <si>
+    <t>Email Verification</t>
+  </si>
+  <si>
+    <t>Session Management</t>
+  </si>
+  <si>
+    <t>Filtering and Sorting</t>
+  </si>
+  <si>
+    <t>Add to Cart</t>
   </si>
   <si>
     <t>Units</t>
@@ -119,16 +107,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹4,435.20</t>
-  </si>
-  <si>
-    <t>₹8,785.92</t>
-  </si>
-  <si>
-    <t>₹532.22</t>
-  </si>
-  <si>
-    <t>₹13,753.34</t>
+    <t>₹5,227.20</t>
+  </si>
+  <si>
+    <t>₹7,772.16</t>
+  </si>
+  <si>
+    <t>₹627.26</t>
+  </si>
+  <si>
+    <t>₹13,626.62</t>
   </si>
 </sst>
 </file>
@@ -489,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -544,13 +532,13 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>0.6000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="I2">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -564,22 +552,22 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="F3">
-        <v>0.8999999999999999</v>
+        <v>0.54</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0.6000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="I3">
-        <v>0.54</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -587,10 +575,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -602,13 +590,13 @@
         <v>0.54</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I4">
-        <v>0.36</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -619,83 +607,83 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="F5">
-        <v>1.26</v>
+        <v>0.36</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I5">
-        <v>0.8999999999999999</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="F6">
-        <v>0.8999999999999999</v>
+        <v>1.26</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>0.6000000000000001</v>
+        <v>2</v>
       </c>
       <c r="I6">
-        <v>0.54</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>0.6000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0.54</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H7">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="I7">
-        <v>0.36</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -703,28 +691,28 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="I8">
-        <v>0.8999999999999999</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -732,164 +720,77 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="I9">
-        <v>1.26</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>6.6</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>5.94</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="H10">
-        <v>0.8</v>
+        <v>9.200000000000001</v>
       </c>
       <c r="I10">
-        <v>0.72</v>
+        <v>8.279999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
       <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>8</v>
-      </c>
-      <c r="H12">
-        <v>1.6</v>
-      </c>
-      <c r="I12">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>28</v>
-      </c>
-      <c r="E13">
-        <v>5.6</v>
-      </c>
-      <c r="F13">
-        <v>5.039999999999999</v>
-      </c>
-      <c r="G13">
-        <v>52</v>
-      </c>
-      <c r="H13">
-        <v>10.4</v>
-      </c>
-      <c r="I13">
-        <v>9.359999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -906,65 +807,65 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>36.96</v>
+        <v>43.56</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>68.64000000000001</v>
+        <v>60.72000000000001</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>5.544</v>
+        <v>6.534000000000001</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -972,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: selenium pipeline in wireframe generator
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>Module</t>
   </si>
@@ -56,7 +56,7 @@
     <t>User Registration</t>
   </si>
   <si>
-    <t>Login</t>
+    <t>User Login</t>
   </si>
   <si>
     <t>Product Listing</t>
@@ -71,13 +71,19 @@
     <t>Email Verification</t>
   </si>
   <si>
+    <t>Password Recovery</t>
+  </si>
+  <si>
     <t>Session Management</t>
   </si>
   <si>
-    <t>Filtering and Sorting</t>
-  </si>
-  <si>
-    <t>Add to Cart</t>
+    <t>Product Search</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Reviews and Ratings</t>
   </si>
   <si>
     <t>Units</t>
@@ -107,16 +113,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹5,227.20</t>
-  </si>
-  <si>
-    <t>₹7,772.16</t>
-  </si>
-  <si>
-    <t>₹627.26</t>
-  </si>
-  <si>
-    <t>₹13,626.62</t>
+    <t>₹6,336.00</t>
+  </si>
+  <si>
+    <t>₹4,899.84</t>
+  </si>
+  <si>
+    <t>₹760.32</t>
+  </si>
+  <si>
+    <t>₹11,996.16</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -532,13 +538,13 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>1.4</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="I2">
-        <v>1.26</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -561,13 +567,13 @@
         <v>0.54</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -575,28 +581,28 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+      <c r="F4">
+        <v>0.72</v>
+      </c>
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>0.6000000000000001</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>0.54</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>0.8</v>
-      </c>
-      <c r="I4">
-        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -607,54 +613,54 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.54</v>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>0.4</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>0.36</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>0.6000000000000001</v>
-      </c>
-      <c r="I5">
-        <v>0.54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="F6">
-        <v>1.26</v>
+        <v>0.36</v>
       </c>
       <c r="G6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="I6">
-        <v>1.8</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -665,25 +671,25 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>1.4</v>
+      </c>
+      <c r="F7">
+        <v>1.26</v>
+      </c>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="G7">
-        <v>7</v>
-      </c>
-      <c r="H7">
-        <v>1.4</v>
-      </c>
-      <c r="I7">
-        <v>1.26</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -691,10 +697,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -706,13 +712,13 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="I8">
-        <v>1.26</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -720,77 +726,135 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>0.6000000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0.54</v>
+        <v>0.36</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="I9">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0.8</v>
+      </c>
+      <c r="F11">
+        <v>0.72</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D10">
-        <v>33</v>
-      </c>
-      <c r="E10">
-        <v>6.6</v>
-      </c>
-      <c r="F10">
-        <v>5.94</v>
-      </c>
-      <c r="G10">
-        <v>46</v>
-      </c>
-      <c r="H10">
-        <v>9.200000000000001</v>
-      </c>
-      <c r="I10">
-        <v>8.279999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>7.2</v>
+      </c>
+      <c r="G12">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>5.799999999999999</v>
+      </c>
+      <c r="I12">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -807,65 +871,65 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2">
-        <v>43.56</v>
+        <v>52.8</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>60.72000000000001</v>
+        <v>38.28</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>6.534000000000001</v>
+        <v>7.920000000000001</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -873,7 +937,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: round numerical values in effort estimation calculations for improved accuracy
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Module</t>
   </si>
@@ -50,6 +50,12 @@
     <t>Product Catalog</t>
   </si>
   <si>
+    <t>Shopping Cart</t>
+  </si>
+  <si>
+    <t>Checkout</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -62,28 +68,70 @@
     <t>Product Listing</t>
   </si>
   <si>
-    <t>Product Details</t>
-  </si>
-  <si>
-    <t>Frontend Implementation</t>
+    <t>Product Search</t>
+  </si>
+  <si>
+    <t>Add to Cart</t>
+  </si>
+  <si>
+    <t>Cart Summary</t>
+  </si>
+  <si>
+    <t>Remove from Cart</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Payment</t>
+  </si>
+  <si>
+    <t>Form Implementation</t>
   </si>
   <si>
     <t>Email Verification</t>
   </si>
   <si>
-    <t>Password Recovery</t>
+    <t>Password Encryption</t>
   </si>
   <si>
     <t>Session Management</t>
   </si>
   <si>
-    <t>Product Search</t>
-  </si>
-  <si>
-    <t>Pagination</t>
-  </si>
-  <si>
-    <t>Reviews and Ratings</t>
+    <t>Product Card Design</t>
+  </si>
+  <si>
+    <t>Filtering and Sorting</t>
+  </si>
+  <si>
+    <t>Search Bar Implementation</t>
+  </si>
+  <si>
+    <t>Autocomplete Suggestions</t>
+  </si>
+  <si>
+    <t>Add Product to Cart</t>
+  </si>
+  <si>
+    <t>Cart Update</t>
+  </si>
+  <si>
+    <t>Product Quantity Display</t>
+  </si>
+  <si>
+    <t>Total Cost Calculation</t>
+  </si>
+  <si>
+    <t>Remove Product from Cart</t>
+  </si>
+  <si>
+    <t>Address Form Implementation</t>
+  </si>
+  <si>
+    <t>Payment Gateway Integration</t>
+  </si>
+  <si>
+    <t>Order Confirmation</t>
   </si>
   <si>
     <t>Units</t>
@@ -113,16 +161,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹6,336.00</t>
-  </si>
-  <si>
-    <t>₹4,899.84</t>
-  </si>
-  <si>
-    <t>₹760.32</t>
+    <t>₹12,038.40</t>
   </si>
   <si>
     <t>₹11,996.16</t>
+  </si>
+  <si>
+    <t>₹1,441.92</t>
+  </si>
+  <si>
+    <t>₹25,476.48</t>
   </si>
 </sst>
 </file>
@@ -483,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -535,16 +583,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.8999999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>0.6000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="I2">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -552,28 +600,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="F3">
         <v>0.54</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I3">
-        <v>0.36</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -581,25 +629,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
       <c r="G4">
         <v>3</v>
       </c>
       <c r="H4">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="I4">
         <v>0.54</v>
@@ -610,28 +658,28 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>0.6000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="F5">
-        <v>0.54</v>
+        <v>0.72</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>0.36</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -639,28 +687,28 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="F6">
-        <v>0.36</v>
+        <v>0.54</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I6">
-        <v>0.36</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -668,19 +716,19 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F7">
-        <v>1.26</v>
+        <v>1.44</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -689,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>0.8999999999999999</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -697,19 +745,19 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="F8">
-        <v>0.8999999999999999</v>
+        <v>1.08</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -726,28 +774,28 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0.36</v>
+        <v>0.9</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>0.4</v>
+        <v>1.2</v>
       </c>
       <c r="I9">
-        <v>0.36</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -755,25 +803,25 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F10">
-        <v>0.8999999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="I10">
         <v>0.54</v>
@@ -781,13 +829,13 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -802,7 +850,7 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <v>0.6000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="I11">
         <v>0.54</v>
@@ -812,49 +860,252 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.9</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0.8</v>
+      </c>
+      <c r="I12">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>0.54</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>0.4</v>
+      </c>
+      <c r="I13">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0.8</v>
+      </c>
+      <c r="F14">
+        <v>0.72</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0.6</v>
+      </c>
+      <c r="I14">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>0.6</v>
+      </c>
+      <c r="F15">
+        <v>0.54</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>0.4</v>
+      </c>
+      <c r="I15">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1.2</v>
+      </c>
+      <c r="F16">
+        <v>1.08</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>0.8</v>
+      </c>
+      <c r="I16">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>1.6</v>
+      </c>
+      <c r="F17">
+        <v>1.44</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>0.6</v>
+      </c>
+      <c r="F18">
+        <v>0.54</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>76</v>
+      </c>
+      <c r="E19">
+        <v>15.2</v>
+      </c>
+      <c r="F19">
+        <v>13.68</v>
+      </c>
+      <c r="G19">
+        <v>71</v>
+      </c>
+      <c r="H19">
+        <v>14.2</v>
+      </c>
+      <c r="I19">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
         <v>40</v>
       </c>
-      <c r="E12">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>7.2</v>
-      </c>
-      <c r="G12">
-        <v>29</v>
-      </c>
-      <c r="H12">
-        <v>5.799999999999999</v>
-      </c>
-      <c r="I12">
-        <v>5.22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" t="s">
-        <v>24</v>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -871,73 +1122,73 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B2">
-        <v>52.8</v>
+        <v>100.32</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B3">
-        <v>38.28</v>
+        <v>93.72</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B4">
-        <v>7.920000000000001</v>
+        <v>15.02</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update effort estimation calculations for improved accuracy and refactor code for better readability
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t>Module</t>
   </si>
@@ -44,94 +44,115 @@
     <t>Backend Testing</t>
   </si>
   <si>
-    <t>User Authentication</t>
-  </si>
-  <si>
-    <t>Product Catalog</t>
-  </si>
-  <si>
-    <t>Shopping Cart</t>
-  </si>
-  <si>
-    <t>Checkout</t>
+    <t>Website</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>User Registration</t>
-  </si>
-  <si>
-    <t>User Login</t>
-  </si>
-  <si>
-    <t>Product Listing</t>
-  </si>
-  <si>
-    <t>Product Search</t>
-  </si>
-  <si>
-    <t>Add to Cart</t>
-  </si>
-  <si>
-    <t>Cart Summary</t>
-  </si>
-  <si>
-    <t>Remove from Cart</t>
-  </si>
-  <si>
-    <t>Shipping Address</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>Form Implementation</t>
-  </si>
-  <si>
-    <t>Email Verification</t>
-  </si>
-  <si>
-    <t>Password Encryption</t>
-  </si>
-  <si>
-    <t>Session Management</t>
-  </si>
-  <si>
-    <t>Product Card Design</t>
-  </si>
-  <si>
-    <t>Filtering and Sorting</t>
-  </si>
-  <si>
-    <t>Search Bar Implementation</t>
-  </si>
-  <si>
-    <t>Autocomplete Suggestions</t>
-  </si>
-  <si>
-    <t>Add Product to Cart</t>
-  </si>
-  <si>
-    <t>Cart Update</t>
-  </si>
-  <si>
-    <t>Product Quantity Display</t>
-  </si>
-  <si>
-    <t>Total Cost Calculation</t>
-  </si>
-  <si>
-    <t>Remove Product from Cart</t>
-  </si>
-  <si>
-    <t>Address Form Implementation</t>
-  </si>
-  <si>
-    <t>Payment Gateway Integration</t>
-  </si>
-  <si>
-    <t>Order Confirmation</t>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>Match Fixtures</t>
+  </si>
+  <si>
+    <t>Match Results</t>
+  </si>
+  <si>
+    <t>Match Centre</t>
+  </si>
+  <si>
+    <t>League Tables</t>
+  </si>
+  <si>
+    <t>News Listing</t>
+  </si>
+  <si>
+    <t>News Article</t>
+  </si>
+  <si>
+    <t>Quizzes</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Content Landing</t>
+  </si>
+  <si>
+    <t>Player Listing</t>
+  </si>
+  <si>
+    <t>Video Hub</t>
+  </si>
+  <si>
+    <t>Partners</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Club Store</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>HR, Hiring, Recruitment and Job Opportunities</t>
+  </si>
+  <si>
+    <t>UI/UX implementation</t>
+  </si>
+  <si>
+    <t>Client-side functionality</t>
+  </si>
+  <si>
+    <t>Display list of upcoming football matches</t>
+  </si>
+  <si>
+    <t>Display results of completed football matches</t>
+  </si>
+  <si>
+    <t>Provide real-time updates and statistics during a football match</t>
+  </si>
+  <si>
+    <t>Display the current standings of football leagues</t>
+  </si>
+  <si>
+    <t>Displays a list of news articles</t>
+  </si>
+  <si>
+    <t>Displays a specific news article with embedded polls</t>
+  </si>
+  <si>
+    <t>Displays multiple-choice quizzes</t>
+  </si>
+  <si>
+    <t>Allows users to search for specific content on the website</t>
+  </si>
+  <si>
+    <t>Displays a specific piece of content, such as a player profile or video</t>
+  </si>
+  <si>
+    <t>Displays a list of football players</t>
+  </si>
+  <si>
+    <t>Displays a collection of football videos</t>
+  </si>
+  <si>
+    <t>Displays information about the club's partners</t>
+  </si>
+  <si>
+    <t>Ensures the website is running smoothly and updates are made regularly</t>
+  </si>
+  <si>
+    <t>Allows users to purchase merchandise related to the football club</t>
+  </si>
+  <si>
+    <t>Displays marketing content related to the football club</t>
+  </si>
+  <si>
+    <t>Displays job opportunities and information about working for the football club</t>
   </si>
   <si>
     <t>Units</t>
@@ -161,16 +182,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹12,038.40</t>
-  </si>
-  <si>
-    <t>₹11,996.16</t>
-  </si>
-  <si>
-    <t>₹1,441.92</t>
-  </si>
-  <si>
-    <t>₹25,476.48</t>
+    <t>₹17,265.60</t>
+  </si>
+  <si>
+    <t>₹10,475.52</t>
+  </si>
+  <si>
+    <t>₹2,071.68</t>
+  </si>
+  <si>
+    <t>₹29,812.80</t>
   </si>
 </sst>
 </file>
@@ -531,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -571,10 +592,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -586,13 +607,13 @@
         <v>0.9</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1.26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -600,28 +621,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F3">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -629,19 +650,19 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0.36</v>
+        <v>0.9</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -658,10 +679,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -673,13 +694,13 @@
         <v>0.72</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I5">
-        <v>0.9</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -687,135 +708,135 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>0.54</v>
+        <v>1.8</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H6">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="I6">
-        <v>0.72</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="F7">
-        <v>1.44</v>
+        <v>1.08</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I7">
-        <v>0.9</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1.08</v>
+        <v>0.9</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="I8">
-        <v>0.72</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F9">
-        <v>0.9</v>
+        <v>0.72</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="I9">
-        <v>1.08</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0.72</v>
+        <v>0.9</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -829,138 +850,138 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>1.2</v>
+      </c>
+      <c r="F11">
+        <v>1.08</v>
+      </c>
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <v>0.8</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>0.72</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>0.6</v>
-      </c>
-      <c r="I11">
-        <v>0.54</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F12">
-        <v>0.9</v>
+        <v>0.72</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="I12">
-        <v>0.72</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <v>0.6</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>0.54</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>0.4</v>
-      </c>
-      <c r="I13">
-        <v>0.36</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1.2</v>
+      </c>
+      <c r="F14">
+        <v>1.08</v>
+      </c>
+      <c r="G14">
         <v>4</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <v>0.8</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>0.72</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>0.6</v>
-      </c>
-      <c r="I14">
-        <v>0.54</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="F15">
-        <v>0.54</v>
+        <v>0.72</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -974,138 +995,167 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>1.6</v>
+      </c>
+      <c r="F16">
+        <v>1.44</v>
+      </c>
+      <c r="G16">
         <v>6</v>
       </c>
-      <c r="E16">
+      <c r="H16">
         <v>1.2</v>
       </c>
-      <c r="F16">
+      <c r="I16">
         <v>1.08</v>
-      </c>
-      <c r="G16">
-        <v>4</v>
-      </c>
-      <c r="H16">
-        <v>0.8</v>
-      </c>
-      <c r="I16">
-        <v>0.72</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E17">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="F17">
-        <v>1.44</v>
+        <v>1.8</v>
       </c>
       <c r="G17">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="I17">
-        <v>1.8</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E18">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F18">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="I18">
-        <v>0.36</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="D19">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>15.2</v>
+        <v>1.6</v>
       </c>
       <c r="F19">
-        <v>13.68</v>
+        <v>1.44</v>
       </c>
       <c r="G19">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="H19">
-        <v>14.2</v>
+        <v>1.2</v>
       </c>
       <c r="I19">
-        <v>12.78</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
       <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" t="s">
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>109</v>
+      </c>
+      <c r="E20">
+        <v>21.8</v>
+      </c>
+      <c r="F20">
+        <v>19.62</v>
+      </c>
+      <c r="G20">
+        <v>62</v>
+      </c>
+      <c r="H20">
+        <v>12.4</v>
+      </c>
+      <c r="I20">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I21" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1129,66 +1179,66 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B2">
-        <v>100.32</v>
+        <v>143.88</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B3">
-        <v>93.72</v>
+        <v>81.84</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B4">
-        <v>15.02</v>
+        <v>21.58</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: implemented GPT-4o model utilization
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>Module</t>
   </si>
@@ -44,115 +44,34 @@
     <t>Backend Testing</t>
   </si>
   <si>
-    <t>Website</t>
+    <t>User Authentication</t>
+  </si>
+  <si>
+    <t>Product Catalog</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Homepage</t>
-  </si>
-  <si>
-    <t>Match Fixtures</t>
-  </si>
-  <si>
-    <t>Match Results</t>
-  </si>
-  <si>
-    <t>Match Centre</t>
-  </si>
-  <si>
-    <t>League Tables</t>
-  </si>
-  <si>
-    <t>News Listing</t>
-  </si>
-  <si>
-    <t>News Article</t>
-  </si>
-  <si>
-    <t>Quizzes</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>Content Landing</t>
-  </si>
-  <si>
-    <t>Player Listing</t>
-  </si>
-  <si>
-    <t>Video Hub</t>
-  </si>
-  <si>
-    <t>Partners</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
-    <t>Club Store</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>HR, Hiring, Recruitment and Job Opportunities</t>
-  </si>
-  <si>
-    <t>UI/UX implementation</t>
-  </si>
-  <si>
-    <t>Client-side functionality</t>
-  </si>
-  <si>
-    <t>Display list of upcoming football matches</t>
-  </si>
-  <si>
-    <t>Display results of completed football matches</t>
-  </si>
-  <si>
-    <t>Provide real-time updates and statistics during a football match</t>
-  </si>
-  <si>
-    <t>Display the current standings of football leagues</t>
-  </si>
-  <si>
-    <t>Displays a list of news articles</t>
-  </si>
-  <si>
-    <t>Displays a specific news article with embedded polls</t>
-  </si>
-  <si>
-    <t>Displays multiple-choice quizzes</t>
-  </si>
-  <si>
-    <t>Allows users to search for specific content on the website</t>
-  </si>
-  <si>
-    <t>Displays a specific piece of content, such as a player profile or video</t>
-  </si>
-  <si>
-    <t>Displays a list of football players</t>
-  </si>
-  <si>
-    <t>Displays a collection of football videos</t>
-  </si>
-  <si>
-    <t>Displays information about the club's partners</t>
-  </si>
-  <si>
-    <t>Ensures the website is running smoothly and updates are made regularly</t>
-  </si>
-  <si>
-    <t>Allows users to purchase merchandise related to the football club</t>
-  </si>
-  <si>
-    <t>Displays marketing content related to the football club</t>
-  </si>
-  <si>
-    <t>Displays job opportunities and information about working for the football club</t>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Product Listing</t>
+  </si>
+  <si>
+    <t>Product Detail</t>
+  </si>
+  <si>
+    <t>Frontend UI/UX Implementation</t>
+  </si>
+  <si>
+    <t>Backend API Implementation</t>
+  </si>
+  <si>
+    <t>Database Integration</t>
   </si>
   <si>
     <t>Units</t>
@@ -182,16 +101,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹17,265.60</t>
-  </si>
-  <si>
-    <t>₹10,475.52</t>
-  </si>
-  <si>
-    <t>₹2,071.68</t>
-  </si>
-  <si>
-    <t>₹29,812.80</t>
+    <t>₹3,168.00</t>
+  </si>
+  <si>
+    <t>₹6,420.48</t>
+  </si>
+  <si>
+    <t>₹380.16</t>
+  </si>
+  <si>
+    <t>₹9,968.64</t>
   </si>
 </sst>
 </file>
@@ -552,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,10 +511,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -607,13 +526,13 @@
         <v>0.9</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -621,28 +540,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1.26</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -653,16 +572,16 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -682,16 +601,16 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="F5">
-        <v>0.72</v>
+        <v>0.54</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -708,126 +627,126 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="F6">
-        <v>1.8</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
       <c r="H6">
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
       <c r="I6">
-        <v>1.44</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="F7">
-        <v>1.08</v>
+        <v>1.26</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>0.72</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="I8">
-        <v>0.54</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H9">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>0.36</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -850,312 +769,80 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1.08</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="I11">
-        <v>0.72</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>3.6</v>
+      </c>
+      <c r="G12">
         <v>38</v>
       </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>0.8</v>
-      </c>
-      <c r="F12">
-        <v>0.72</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
       <c r="H12">
-        <v>0.4</v>
+        <v>7.6</v>
       </c>
       <c r="I12">
-        <v>0.36</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
       <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0.9</v>
-      </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-      <c r="H13">
-        <v>0.6</v>
-      </c>
-      <c r="I13">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>1.2</v>
-      </c>
-      <c r="F14">
-        <v>1.08</v>
-      </c>
-      <c r="G14">
-        <v>4</v>
-      </c>
-      <c r="H14">
-        <v>0.8</v>
-      </c>
-      <c r="I14">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>0.8</v>
-      </c>
-      <c r="F15">
-        <v>0.72</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>0.4</v>
-      </c>
-      <c r="I15">
-        <v>0.36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>1.6</v>
-      </c>
-      <c r="F16">
-        <v>1.44</v>
-      </c>
-      <c r="G16">
-        <v>6</v>
-      </c>
-      <c r="H16">
-        <v>1.2</v>
-      </c>
-      <c r="I16">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>1.8</v>
-      </c>
-      <c r="G17">
-        <v>6</v>
-      </c>
-      <c r="H17">
-        <v>1.2</v>
-      </c>
-      <c r="I17">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-      <c r="E18">
-        <v>1.4</v>
-      </c>
-      <c r="F18">
-        <v>1.26</v>
-      </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18">
-        <v>0.8</v>
-      </c>
-      <c r="I18">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>1.6</v>
-      </c>
-      <c r="F19">
-        <v>1.44</v>
-      </c>
-      <c r="G19">
-        <v>6</v>
-      </c>
-      <c r="H19">
-        <v>1.2</v>
-      </c>
-      <c r="I19">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20">
-        <v>109</v>
-      </c>
-      <c r="E20">
-        <v>21.8</v>
-      </c>
-      <c r="F20">
-        <v>19.62</v>
-      </c>
-      <c r="G20">
-        <v>62</v>
-      </c>
-      <c r="H20">
-        <v>12.4</v>
-      </c>
-      <c r="I20">
-        <v>11.16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" t="s">
-        <v>47</v>
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1174,71 +861,71 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>143.88</v>
+        <v>26.4</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>81.84</v>
+        <v>50.16</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B4">
-        <v>21.58</v>
+        <v>3.96</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: update JSON serialization in prompt generation to handle non-serializable objects
</commit_message>
<xml_diff>
--- a/effort_estimation.xlsx
+++ b/effort_estimation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>Module</t>
   </si>
@@ -44,34 +44,91 @@
     <t>Backend Testing</t>
   </si>
   <si>
-    <t>User Authentication</t>
-  </si>
-  <si>
-    <t>Product Catalog</t>
+    <t>AI-Powered Proficiency Assessment</t>
+  </si>
+  <si>
+    <t>Adaptive Lesson Planning</t>
+  </si>
+  <si>
+    <t>Conversational AI for Real-Life Dialogues</t>
+  </si>
+  <si>
+    <t>Spaced Repetition &amp; Revision Scheduling</t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>User Registration</t>
-  </si>
-  <si>
-    <t>User Login</t>
-  </si>
-  <si>
-    <t>Product Listing</t>
-  </si>
-  <si>
-    <t>Product Detail</t>
-  </si>
-  <si>
-    <t>Frontend UI/UX Implementation</t>
-  </si>
-  <si>
-    <t>Backend API Implementation</t>
-  </si>
-  <si>
-    <t>Database Integration</t>
+    <t>Diagnostic Test at Onboarding</t>
+  </si>
+  <si>
+    <t>Ongoing Performance Analysis</t>
+  </si>
+  <si>
+    <t>Personalized Lesson Plans</t>
+  </si>
+  <si>
+    <t>Interactive Lesson Display</t>
+  </si>
+  <si>
+    <t>Real-World Conversation Simulation</t>
+  </si>
+  <si>
+    <t>Pronunciation Feedback</t>
+  </si>
+  <si>
+    <t>Revision Scheduling</t>
+  </si>
+  <si>
+    <t>Lesson Summaries</t>
+  </si>
+  <si>
+    <t>Diagnostic Test Implementation</t>
+  </si>
+  <si>
+    <t>Proficiency Level Evaluation</t>
+  </si>
+  <si>
+    <t>User Performance Tracking</t>
+  </si>
+  <si>
+    <t>Proficiency Level Adjustment</t>
+  </si>
+  <si>
+    <t>User Weak Area Identification</t>
+  </si>
+  <si>
+    <t>Lesson Plan Generation</t>
+  </si>
+  <si>
+    <t>Lesson Layout Design</t>
+  </si>
+  <si>
+    <t>Lesson Interactivity Implementation</t>
+  </si>
+  <si>
+    <t>Conversation Scenario Design</t>
+  </si>
+  <si>
+    <t>Conversation Implementation</t>
+  </si>
+  <si>
+    <t>Pronunciation Analysis</t>
+  </si>
+  <si>
+    <t>Feedback Generation</t>
+  </si>
+  <si>
+    <t>Spaced Repetition Algorithm Implementation</t>
+  </si>
+  <si>
+    <t>Scheduling User Reviews</t>
+  </si>
+  <si>
+    <t>Summary Generation</t>
+  </si>
+  <si>
+    <t>Summary Presentation</t>
   </si>
   <si>
     <t>Units</t>
@@ -101,16 +158,16 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>₹3,168.00</t>
-  </si>
-  <si>
-    <t>₹6,420.48</t>
-  </si>
-  <si>
-    <t>₹380.16</t>
-  </si>
-  <si>
-    <t>₹9,968.64</t>
+    <t>₹19,641.60</t>
+  </si>
+  <si>
+    <t>₹22,302.72</t>
+  </si>
+  <si>
+    <t>₹2,357.76</t>
+  </si>
+  <si>
+    <t>₹44,302.08</t>
   </si>
 </sst>
 </file>
@@ -471,7 +528,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -511,28 +568,28 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="F2">
-        <v>0.9</v>
+        <v>1.26</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="I2">
-        <v>0.54</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -540,28 +597,28 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="I3">
-        <v>0.9</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -569,28 +626,28 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
       <c r="I4">
-        <v>0.54</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -598,57 +655,57 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="I5">
-        <v>0.36</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
+        <v>1.4</v>
       </c>
       <c r="I6">
-        <v>0.36</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -656,28 +713,28 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F7">
-        <v>1.26</v>
+        <v>1.44</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7">
-        <v>0.9</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -685,28 +742,28 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>1.4</v>
+        <v>0.4</v>
       </c>
       <c r="I8">
-        <v>1.26</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -714,135 +771,309 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="I9">
-        <v>0.9</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>0.9</v>
+        <v>1.8</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H10">
-        <v>0.6</v>
+        <v>2.4</v>
       </c>
       <c r="I10">
-        <v>0.54</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
         <v>3</v>
       </c>
-      <c r="H11">
-        <v>0.6</v>
-      </c>
       <c r="I11">
-        <v>0.54</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>1.4</v>
+      </c>
+      <c r="F12">
+        <v>1.26</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>1.8</v>
+      </c>
+      <c r="I12">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>1.4</v>
+      </c>
+      <c r="I13">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>3.6</v>
-      </c>
-      <c r="G12">
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>1.6</v>
+      </c>
+      <c r="F14">
+        <v>1.44</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1.2</v>
+      </c>
+      <c r="F15">
+        <v>1.08</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>1.6</v>
+      </c>
+      <c r="I15">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>1.4</v>
+      </c>
+      <c r="F16">
+        <v>1.26</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>1.8</v>
+      </c>
+      <c r="I16">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0.9</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>1.4</v>
+      </c>
+      <c r="I17">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>124</v>
+      </c>
+      <c r="E18">
+        <v>24.8</v>
+      </c>
+      <c r="F18">
+        <v>22.32</v>
+      </c>
+      <c r="G18">
+        <v>132</v>
+      </c>
+      <c r="H18">
+        <v>26.4</v>
+      </c>
+      <c r="I18">
+        <v>23.76000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="H12">
-        <v>7.6</v>
-      </c>
-      <c r="I12">
-        <v>6.84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" t="s">
-        <v>20</v>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -861,71 +1092,71 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>26.4</v>
+        <v>163.68</v>
       </c>
       <c r="C2">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>50.16</v>
+        <v>174.24</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B4">
-        <v>3.96</v>
+        <v>24.56</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>